<commit_message>
Last added data (tests)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,11 +3,10 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="measured_current">Sheet1!$A:$A</definedName>
@@ -415,28 +414,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -760,6 +741,999 @@
         <v>8</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.000396729</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.000244141</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.000137329</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.000366211</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.000366211</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.000396729</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.000396729</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.000137329</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.000396729</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.000396729</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B42" t="n">
+        <v>6.10352e-05</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B59" t="n">
+        <v>6.10352e-05</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>3</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.000366211</v>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>0.000244141</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.00120544</v>
+      </c>
+      <c r="D95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B99" t="n">
+        <v>6.10352e-05</v>
+      </c>
+      <c r="D99" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.00112915</v>
+      </c>
+      <c r="D100" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.000747681</v>
+      </c>
+      <c r="D101" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+      <c r="D105" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0.000549316</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1.79372</v>
+      </c>
+      <c r="B116" t="n">
+        <v>13.1575</v>
+      </c>
+      <c r="D116" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B117" t="n">
+        <v>13.1681</v>
+      </c>
+      <c r="D117" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B118" t="n">
+        <v>13.1421</v>
+      </c>
+      <c r="D118" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>0.000701904</v>
+      </c>
+      <c r="B119" t="n">
+        <v>13.1421</v>
+      </c>
+      <c r="C119" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add hearder and delete old tests
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="measured_current">Sheet1!$A:$A</definedName>
@@ -18,11 +19,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <color rgb="FF0070C0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF0070C0"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -47,8 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,9 +432,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1734,7 +1752,69 @@
         <v>4</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>00000000</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>serial num</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Voltage</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>CV</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>67362781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct header and delete old tests
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,14 +12,14 @@
   <definedNames>
     <definedName name="measured_current">Sheet1!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,6 +37,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF0070C0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -61,12 +69,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,44 +1782,348 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="14.77734375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.5546875" customWidth="1" min="3" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14.21875" customWidth="1" min="6" max="6"/>
+    <col width="22.77734375" customWidth="1" min="7" max="7"/>
+    <col width="21.44140625" customWidth="1" min="8" max="8"/>
+    <col width="18.33203125" customWidth="1" min="9" max="9"/>
+    <col width="17.5546875" customWidth="1" min="10" max="10"/>
+    <col width="16.5546875" customWidth="1" min="11" max="11"/>
+    <col width="15.5546875" customWidth="1" min="12" max="12"/>
+    <col width="15.21875" customWidth="1" min="13" max="13"/>
+    <col width="16.33203125" customWidth="1" min="14" max="14"/>
+    <col width="29.44140625" customWidth="1" min="15" max="15"/>
+    <col width="26.88671875" customWidth="1" min="16" max="16"/>
+    <col width="18.109375" customWidth="1" min="17" max="17"/>
+    <col width="14" customWidth="1" min="18" max="18"/>
+    <col width="12.44140625" customWidth="1" min="19" max="19"/>
+    <col width="15.109375" customWidth="1" min="20" max="20"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>serial num</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Current</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Voltage</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Data exported from PV-test-bench: 20160429-00h00m</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>67362781</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Module Number</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pmpp</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Uoc</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Isc</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Temperature Ambient</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Temperature Lamps</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Pmpp Reference</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Pmpp Deviation</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Uoc Reference</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Uoc Deviation</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Isc Reference</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Isc Deviation</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Temperature Ambient Reference</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Temperature Lamps Reference</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Reference Number</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>31.0654</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>9.933199999999999</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4.3456</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>07/18/2024</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>13:46:06</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>312</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>31.0654</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.933199999999999</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4.3456</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>07/18/2024</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>13:46:44</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>313</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>31.0654</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9.933199999999999</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4.3456</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>07/18/2024</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>13:48:15</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>